<commit_message>
Updated Sprint Planning (mostly formatting)
</commit_message>
<xml_diff>
--- a/SprintPlanning/INFO-5139-Sprint Planning Meeting 1.0.xlsx
+++ b/SprintPlanning/INFO-5139-Sprint Planning Meeting 1.0.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/117c460ab79249a6/Work/Fanshawe/Courses/INFO-5139-Application-Project/2022_Winter/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepp\Documents\GitHub\ApplicationProjectGroup1\SprintPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{A7296D7D-5132-498E-80ED-362BC040A48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76B1F570-FF73-4DF5-8ACC-84E892BDDDB9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C088F75-E902-4425-927E-EF8672F27543}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="1680" windowWidth="21600" windowHeight="11385" xr2:uid="{C9C5D2BF-3AE6-4156-8BB2-695A131DFF04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28320" windowHeight="11115" activeTab="1" xr2:uid="{C9C5D2BF-3AE6-4156-8BB2-695A131DFF04}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
     <sheet name="Current Sprint" sheetId="2" r:id="rId2"/>
     <sheet name="Technology" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,10 +25,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Row #</t>
   </si>
@@ -71,9 +67,6 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>##</t>
-  </si>
-  <si>
     <t>Attendees (Last name, First Name)</t>
   </si>
   <si>
@@ -87,24 +80,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Student 1</t>
-  </si>
-  <si>
-    <t>Student 2</t>
-  </si>
-  <si>
-    <t>We tried to contact him using email and discussion board with no success.</t>
-  </si>
-  <si>
-    <t>Student 3</t>
-  </si>
-  <si>
-    <t>Sprint Planning Meeting ##</t>
-  </si>
-  <si>
-    <t>Sprint ##</t>
   </si>
   <si>
     <t>Complexity and number of items must be reasonable according to the number of team members.</t>
@@ -174,25 +149,13 @@
     <t>Front End Technology?</t>
   </si>
   <si>
-    <t>i.e. Angular, React, Laravel, Pure PHP, etc.</t>
-  </si>
-  <si>
     <t>Are you using or plan to use a Data Base?</t>
   </si>
   <si>
-    <t>Yes/No</t>
-  </si>
-  <si>
     <t>If Yes which DB engine are you using?</t>
   </si>
   <si>
-    <t>i.e. MariaDB, Mysql, Mongo DB, etc.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Which application server are you using? </t>
-  </si>
-  <si>
-    <t>i.e. Apache, Nodejs, Nginx, etc.</t>
   </si>
   <si>
     <t>Describe here any additional technologies</t>
@@ -225,6 +188,68 @@
         <scheme val="minor"/>
       </rPr>
       <t>You can as change column names to match your format as needed.</t>
+    </r>
+  </si>
+  <si>
+    <t>Mokhurenko, Yaroslav</t>
+  </si>
+  <si>
+    <t>Derbishev, Temirlan</t>
+  </si>
+  <si>
+    <t>Diaz-Vargas, Nicolas</t>
+  </si>
+  <si>
+    <t>Patel, Jay</t>
+  </si>
+  <si>
+    <t>Bikov, Aleksei</t>
+  </si>
+  <si>
+    <t>Sprint Planning Meeting 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i.e. Apache, Nodejs, Nginx, etc.
+</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">i.e. Angular, React, Laravel, Pure PHP, etc.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>React</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">i.e. MariaDB, Mysql, Mongo DB, etc.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Firebase</t>
     </r>
   </si>
 </sst>
@@ -338,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -377,6 +402,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D1333C-4938-4EF8-8EA3-085671C5CE7F}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,7 +821,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="16" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -804,73 +835,86 @@
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>11</v>
+      <c r="B2" s="9">
+        <v>1</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8"/>
       <c r="F2" s="11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="F3" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -889,12 +933,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A875DEB-4808-4559-B6A0-559BDD9EE661}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="32" style="4" customWidth="1"/>
@@ -908,7 +953,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -917,7 +962,7 @@
         <v>9</v>
       </c>
       <c r="G1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>10</v>
@@ -925,10 +970,10 @@
     </row>
     <row r="2" spans="1:11" ht="61.5" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1132,7 +1177,7 @@
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,53 +1188,53 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>34</v>
+        <v>24</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C7" s="14"/>
     </row>
     <row r="8" spans="2:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C8" s="14"/>
     </row>

</xml_diff>

<commit_message>
add nginx as technology
</commit_message>
<xml_diff>
--- a/SprintPlanning/INFO-5139-Sprint Planning Meeting 1.0.xlsx
+++ b/SprintPlanning/INFO-5139-Sprint Planning Meeting 1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepp\Documents\GitHub\ApplicationProjectGroup1\SprintPlanning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University\SEMESTER_4\INFO-5139-APPLICATION_PROJECT\ApplicationProjectGroup1\SprintPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C088F75-E902-4425-927E-EF8672F27543}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F9B165-BBDC-42A8-9249-7A75B571BFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28320" windowHeight="11115" activeTab="1" xr2:uid="{C9C5D2BF-3AE6-4156-8BB2-695A131DFF04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C9C5D2BF-3AE6-4156-8BB2-695A131DFF04}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Row #</t>
   </si>
@@ -209,10 +209,6 @@
     <t>Sprint Planning Meeting 1</t>
   </si>
   <si>
-    <t xml:space="preserve">i.e. Apache, Nodejs, Nginx, etc.
-</t>
-  </si>
-  <si>
     <t>Sprint 1</t>
   </si>
   <si>
@@ -252,12 +248,39 @@
       <t>Firebase</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">i.e. Apache, Nodejs, Nginx, etc.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nginx</t>
+    </r>
+  </si>
+  <si>
+    <t>any AWS free tier services?</t>
+  </si>
+  <si>
+    <t>ReactJS additional packages, e.g. axios for http requsts to endpoints.</t>
+  </si>
+  <si>
+    <t>Everyone should draw their draft of the design for the app and choose the best one on the next meeting.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,6 +359,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -400,14 +432,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,7 +837,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,12 +852,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="F1" s="10" t="s">
         <v>10</v>
       </c>
@@ -866,12 +898,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>17</v>
@@ -934,7 +969,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +978,7 @@
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="32" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="28" style="4" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
@@ -953,7 +988,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1177,12 +1212,12 @@
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="89" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1198,45 +1233,49 @@
       <c r="B3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>41</v>
+      <c r="C3" s="16" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>40</v>
+      <c r="C4" s="17" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>42</v>
+      <c r="C5" s="16" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>38</v>
+      <c r="C6" s="16" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="14" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="2:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update INFO-5139-Sprint Planning Meeting 1.0.xlsx
</commit_message>
<xml_diff>
--- a/SprintPlanning/INFO-5139-Sprint Planning Meeting 1.0.xlsx
+++ b/SprintPlanning/INFO-5139-Sprint Planning Meeting 1.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University\SEMESTER_4\INFO-5139-APPLICATION_PROJECT\ApplicationProjectGroup1\SprintPlanning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepp\Documents\GitHub\ApplicationProjectGroup1\SprintPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F9B165-BBDC-42A8-9249-7A75B571BFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C97CBBA-CBDC-453E-A52B-1B2E4CDBA644}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C9C5D2BF-3AE6-4156-8BB2-695A131DFF04}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
   <si>
     <t>Row #</t>
   </si>
@@ -267,13 +267,91 @@
     </r>
   </si>
   <si>
-    <t>any AWS free tier services?</t>
-  </si>
-  <si>
     <t>ReactJS additional packages, e.g. axios for http requsts to endpoints.</t>
   </si>
   <si>
     <t>Everyone should draw their draft of the design for the app and choose the best one on the next meeting.</t>
+  </si>
+  <si>
+    <t>Maybe some AWS free tier services</t>
+  </si>
+  <si>
+    <t>FYF-1</t>
+  </si>
+  <si>
+    <t>FYF-2</t>
+  </si>
+  <si>
+    <t>FYF-10</t>
+  </si>
+  <si>
+    <t>FYF-13</t>
+  </si>
+  <si>
+    <t>FYF-15</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Register in the app</t>
+  </si>
+  <si>
+    <t>Edit my profile</t>
+  </si>
+  <si>
+    <t>Fill in details about myself (Name, Gender, Age, College/University, Country of origin etc).</t>
+  </si>
+  <si>
+    <t>Continue to creating my profile</t>
+  </si>
+  <si>
+    <t>Complete creating my profile</t>
+  </si>
+  <si>
+    <t>Maintain the accuracy of my personal</t>
+  </si>
+  <si>
+    <t>Create a post on my page</t>
+  </si>
+  <si>
+    <t>Share content with my friendlist</t>
+  </si>
+  <si>
+    <t>Fast sign up with google account</t>
+  </si>
+  <si>
+    <t>Faster/easier sign up</t>
+  </si>
+  <si>
+    <t>Login into account</t>
+  </si>
+  <si>
+    <t>Have access to my account</t>
+  </si>
+  <si>
+    <t>Share my current status</t>
+  </si>
+  <si>
+    <t>So people know what I am up to</t>
+  </si>
+  <si>
+    <t>Create a burger menu for mobile view</t>
+  </si>
+  <si>
+    <t>For people coming to site from mobiles</t>
+  </si>
+  <si>
+    <t>FYF-33</t>
+  </si>
+  <si>
+    <t>FYF-34</t>
+  </si>
+  <si>
+    <t>FYF-39</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -447,6 +525,9 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -454,9 +535,6 @@
         <b/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -492,6 +570,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>164540</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>106412</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE6359A6-02FF-4F73-8E54-3170A0F2226B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5029200"/>
+          <a:ext cx="18738290" cy="11726912"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8BEDA70-9192-4B0F-ADAD-6D5843AC9319}" name="Table1" displayName="Table1" ref="A4:D12" totalsRowShown="0">
   <autoFilter ref="A4:D12" xr:uid="{D6E6D6F8-0326-4209-932F-132751BAFD32}"/>
@@ -514,10 +641,10 @@
     <tableColumn id="3" xr3:uid="{865EC776-2CD0-4898-A780-7D922EA779A4}" name="As a/an" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{D4693A27-1AE0-42E7-B1EA-6C949553AD36}" name="I want to…" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{F573B293-2938-4D1E-BA0F-785E925271E1}" name="so that…" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{6E003B49-3338-453C-8B4E-0924371B0613}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{6E003B49-3338-453C-8B4E-0924371B0613}" name="Notes" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{E1CC7E03-DDEE-4F57-B64E-8BAEF7BB58F9}" name="Priority"/>
     <tableColumn id="8" xr3:uid="{E2AE2732-3383-4169-996C-89A839547578}" name="Status"/>
-    <tableColumn id="9" xr3:uid="{8497112C-097A-4F3A-B978-3B95BE47AA2B}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{8497112C-097A-4F3A-B978-3B95BE47AA2B}" name="Owner" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -530,8 +657,8 @@
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{21E6774A-F1DF-4758-B652-496665FB2BE3}" name="Questions:" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{62F92012-F289-413A-92F3-814F6F0636AE}" name="Answers" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{21E6774A-F1DF-4758-B652-496665FB2BE3}" name="Questions:" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{62F92012-F289-413A-92F3-814F6F0636AE}" name="Answers" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -837,7 +964,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +1033,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>17</v>
@@ -958,8 +1085,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -969,7 +1097,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,40 +1172,160 @@
       <c r="A5">
         <v>1</v>
       </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1266,7 +1514,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,7 +1522,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed unused columns from Current Sprint
</commit_message>
<xml_diff>
--- a/SprintPlanning/INFO-5139-Sprint Planning Meeting 1.0.xlsx
+++ b/SprintPlanning/INFO-5139-Sprint Planning Meeting 1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepp\Documents\GitHub\ApplicationProjectGroup1\SprintPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C97CBBA-CBDC-453E-A52B-1B2E4CDBA644}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9911D356-0148-4322-871F-3A2ED418808E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C9C5D2BF-3AE6-4156-8BB2-695A131DFF04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9C5D2BF-3AE6-4156-8BB2-695A131DFF04}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>Row #</t>
   </si>
@@ -49,16 +49,7 @@
     <t>so that…</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Owner</t>
   </si>
   <si>
     <t>Group Number:</t>
@@ -523,10 +514,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -535,9 +523,6 @@
         <b/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -625,26 +610,23 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9A3D94CC-586F-4DB3-9D36-6D516D4DD278}" name="Attendees (Last name, First Name)"/>
     <tableColumn id="2" xr3:uid="{F76AAE24-59EF-41BA-967E-22D40F01C930}" name="Present"/>
-    <tableColumn id="3" xr3:uid="{56ABFB7A-02EA-4C86-9F19-F400E986A325}" name="Absent" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{7652999F-1C7B-410D-9D19-756921E86A91}" name="Notes/Comments" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{56ABFB7A-02EA-4C86-9F19-F400E986A325}" name="Absent" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{7652999F-1C7B-410D-9D19-756921E86A91}" name="Notes/Comments" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1F24383E-81C1-48AA-B3CE-0A4651C21888}" name="Table13" displayName="Table13" ref="A4:I34" totalsRowShown="0">
-  <autoFilter ref="A4:I34" xr:uid="{6A4555D3-6CFC-4813-9C18-EEC3122BBE8B}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1F24383E-81C1-48AA-B3CE-0A4651C21888}" name="Table13" displayName="Table13" ref="A4:F12" totalsRowShown="0">
+  <autoFilter ref="A4:F12" xr:uid="{6A4555D3-6CFC-4813-9C18-EEC3122BBE8B}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6C40B138-5F4F-4627-81B5-6CCFB7600CDB}" name="Row #"/>
-    <tableColumn id="2" xr3:uid="{615EA2A2-FE7A-4D9C-9A42-7FA8DC77F155}" name="ID" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{865EC776-2CD0-4898-A780-7D922EA779A4}" name="As a/an" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{D4693A27-1AE0-42E7-B1EA-6C949553AD36}" name="I want to…" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{F573B293-2938-4D1E-BA0F-785E925271E1}" name="so that…" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{6E003B49-3338-453C-8B4E-0924371B0613}" name="Notes" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{E1CC7E03-DDEE-4F57-B64E-8BAEF7BB58F9}" name="Priority"/>
+    <tableColumn id="2" xr3:uid="{615EA2A2-FE7A-4D9C-9A42-7FA8DC77F155}" name="ID" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{865EC776-2CD0-4898-A780-7D922EA779A4}" name="As a/an" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{D4693A27-1AE0-42E7-B1EA-6C949553AD36}" name="I want to…" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{F573B293-2938-4D1E-BA0F-785E925271E1}" name="so that…" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{E2AE2732-3383-4169-996C-89A839547578}" name="Status"/>
-    <tableColumn id="9" xr3:uid="{8497112C-097A-4F3A-B978-3B95BE47AA2B}" name="Owner" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -657,8 +639,8 @@
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{21E6774A-F1DF-4758-B652-496665FB2BE3}" name="Questions:" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{62F92012-F289-413A-92F3-814F6F0636AE}" name="Answers" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{21E6774A-F1DF-4758-B652-496665FB2BE3}" name="Questions:" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{62F92012-F289-413A-92F3-814F6F0636AE}" name="Answers" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -963,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D1333C-4938-4EF8-8EA3-085671C5CE7F}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,19 +962,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
       <c r="F1" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="33.75" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -1000,83 +982,83 @@
       <c r="C2" s="7"/>
       <c r="D2" s="8"/>
       <c r="F2" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="F3" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1094,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A875DEB-4808-4559-B6A0-559BDD9EE661}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,27 +1098,27 @@
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="F1" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G1">
         <v>1</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="61.5" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1155,295 +1137,203 @@
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="H4" s="4"/>
+      <c r="I4"/>
+      <c r="K4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>71</v>
-      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5"/>
+      <c r="K5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" t="s">
-        <v>71</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6"/>
+      <c r="K6"/>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" t="s">
-        <v>71</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7"/>
+      <c r="K7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" t="s">
-        <v>71</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8"/>
+      <c r="K8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" t="s">
-        <v>71</v>
-      </c>
+      <c r="H9" s="4"/>
+      <c r="I9"/>
+      <c r="K9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" t="s">
-        <v>71</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10"/>
+      <c r="K10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" t="s">
-        <v>71</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11"/>
+      <c r="K11"/>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>30</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12"/>
+      <c r="K12"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{D5E28F0E-7D6B-453A-BE92-021A9AAE5A60}">
       <formula1>"00, 01, 02, 03, 04, 05, 06, 07, 08, 09"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H34" xr:uid="{06EE48CD-350C-407D-8C90-E0AF6D94DA36}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F12" xr:uid="{06EE48CD-350C-407D-8C90-E0AF6D94DA36}">
       <formula1>"In Progress, On Hold, Testing, Done, Cancelled"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1471,58 +1361,58 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Agile Board screenshot
Added more columns to Board to match grading rubric for the assignment
</commit_message>
<xml_diff>
--- a/SprintPlanning/INFO-5139-Sprint Planning Meeting 1.0.xlsx
+++ b/SprintPlanning/INFO-5139-Sprint Planning Meeting 1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepp\Documents\GitHub\ApplicationProjectGroup1\SprintPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9911D356-0148-4322-871F-3A2ED418808E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DC64AC-40FB-4B53-A5C5-459FCF51755D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9C5D2BF-3AE6-4156-8BB2-695A131DFF04}"/>
   </bookViews>
@@ -561,21 +561,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>164540</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>106412</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>279622</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>182755</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE6359A6-02FF-4F73-8E54-3170A0F2226B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1865B288-2656-417A-9DBA-6BD57037DB85}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -591,8 +591,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="5029200"/>
-          <a:ext cx="18738290" cy="11726912"/>
+          <a:off x="0" y="4838700"/>
+          <a:ext cx="24339772" cy="12755755"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -946,7 +946,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>